<commit_message>
added LIFO, FIFO, HIFO, and method for each year
</commit_message>
<xml_diff>
--- a/workbooks/after-sales.xlsx
+++ b/workbooks/after-sales.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,7 +516,7 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="n">
-        <v>45345</v>
+        <v>45345.19027777778</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="n">
-        <v>45327</v>
+        <v>45327.97185185185</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -548,7 +548,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="n">
-        <v>45320</v>
+        <v>45320.48010416667</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -564,7 +564,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="n">
-        <v>45281</v>
+        <v>45281.83146990741</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -580,7 +580,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="n">
-        <v>45266</v>
+        <v>45266.91903935185</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -596,7 +596,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="n">
-        <v>45247</v>
+        <v>45247.9331712963</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -612,7 +612,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="n">
-        <v>45243</v>
+        <v>45243.92203703704</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -628,7 +628,7 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="n">
-        <v>45230</v>
+        <v>45230.47232638889</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -644,7 +644,7 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="n">
-        <v>45224</v>
+        <v>45224.69118055556</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -660,7 +660,7 @@
     </row>
     <row r="11">
       <c r="A11" s="4" t="n">
-        <v>45219</v>
+        <v>45219.75883101852</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -676,7 +676,7 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="n">
-        <v>45146</v>
+        <v>45146.03603009259</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -684,15 +684,15 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>383.594323</v>
+        <v>470.261323</v>
       </c>
       <c r="D12" t="n">
-        <v>21.45</v>
+        <v>26.55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="n">
-        <v>45146</v>
+        <v>45146.03285879629</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -700,31 +700,31 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>43834.38366132</v>
+        <v>43801.36281517</v>
       </c>
       <c r="D13" t="n">
-        <v>2563.87</v>
+        <v>2561.94</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="n">
-        <v>45146</v>
+        <v>45131.44159722222</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>53.64615385</v>
+        <v>1418.744626</v>
       </c>
       <c r="D14" t="n">
-        <v>3.17</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="n">
-        <v>45131</v>
+        <v>45124.80702546296</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -732,15 +732,15 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1418.744626</v>
+        <v>922.768313</v>
       </c>
       <c r="D15" t="n">
-        <v>1000</v>
+        <v>674.8200000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="n">
-        <v>45124</v>
+        <v>45124.77539351852</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -748,15 +748,15 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>922.768313</v>
+        <v>941.043309</v>
       </c>
       <c r="D16" t="n">
-        <v>674.8200000000001</v>
+        <v>681.5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="n">
-        <v>45124</v>
+        <v>45124.75659722222</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -764,31 +764,31 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>941.043309</v>
+        <v>971.856015</v>
       </c>
       <c r="D17" t="n">
-        <v>681.5</v>
+        <v>725.9400000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="n">
-        <v>45124</v>
+        <v>45087.11783564815</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>971.856015</v>
+        <v>130.2443386</v>
       </c>
       <c r="D18" t="n">
-        <v>725.9400000000001</v>
+        <v>6.31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="n">
-        <v>45087</v>
+        <v>45067.3153125</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -796,15 +796,15 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>130.2443386</v>
+        <v>58.46972882</v>
       </c>
       <c r="D19" t="n">
-        <v>6.31</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="n">
-        <v>45067</v>
+        <v>45058.33905092593</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -812,31 +812,31 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>58.46972882</v>
+        <v>283.8796531</v>
       </c>
       <c r="D20" t="n">
-        <v>3.1</v>
+        <v>14.59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n">
-        <v>45058</v>
+        <v>45058.19652777778</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>283.8796531</v>
+        <v>44.590986</v>
       </c>
       <c r="D21" t="n">
-        <v>14.59</v>
+        <v>19.13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="n">
-        <v>45058</v>
+        <v>45054.77490740741</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -844,47 +844,47 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>44.590986</v>
+        <v>113.287</v>
       </c>
       <c r="D22" t="n">
-        <v>19.13</v>
+        <v>51.02</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n">
-        <v>45054</v>
+        <v>45014.81280092592</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>113.287</v>
+        <v>6.45060194</v>
       </c>
       <c r="D23" t="n">
-        <v>51.02</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="n">
-        <v>45014</v>
+        <v>45013.15342592593</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>6.45060194</v>
+        <v>2066.699516</v>
       </c>
       <c r="D24" t="n">
-        <v>0.38</v>
+        <v>992.3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="n">
-        <v>45013</v>
+        <v>45012.1265162037</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -892,15 +892,15 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>2066.699516</v>
+        <v>805.484107</v>
       </c>
       <c r="D25" t="n">
-        <v>992.3</v>
+        <v>361.53</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="n">
-        <v>45012</v>
+        <v>45010.50967592592</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -908,15 +908,15 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>805.484107</v>
+        <v>219.938426</v>
       </c>
       <c r="D26" t="n">
-        <v>361.53</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="n">
-        <v>45010</v>
+        <v>45006.65659722222</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -924,31 +924,31 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>219.938426</v>
+        <v>1152.377951</v>
       </c>
       <c r="D27" t="n">
-        <v>100</v>
+        <v>503.82</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="n">
-        <v>45006</v>
+        <v>45005.71923611111</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1152.377951</v>
+        <v>317.43499761</v>
       </c>
       <c r="D28" t="n">
-        <v>503.82</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="n">
-        <v>45005</v>
+        <v>44998.83645833333</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -956,7 +956,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>317.43499761</v>
+        <v>309.67942733</v>
       </c>
       <c r="D29" t="n">
         <v>20</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="n">
-        <v>44998</v>
+        <v>44995.76827546296</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -972,15 +972,15 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>309.67942733</v>
+        <v>10127.87723785</v>
       </c>
       <c r="D30" t="n">
-        <v>20</v>
+        <v>600</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="n">
-        <v>44995</v>
+        <v>44991.70733796297</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -988,15 +988,15 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>10127.87723785</v>
+        <v>311.96112243</v>
       </c>
       <c r="D31" t="n">
-        <v>600</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="n">
-        <v>44991</v>
+        <v>44987.0953125</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1004,15 +1004,15 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>311.96112243</v>
+        <v>12639.46303323</v>
       </c>
       <c r="D32" t="n">
-        <v>20</v>
+        <v>872.4299999999999</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="n">
-        <v>44987</v>
+        <v>44984.69497685185</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1020,15 +1020,15 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>12639.46303323</v>
+        <v>274.33140336</v>
       </c>
       <c r="D33" t="n">
-        <v>872.4299999999999</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="n">
-        <v>44984</v>
+        <v>44963.71480324074</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1036,15 +1036,15 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>274.33140336</v>
+        <v>264.01674599</v>
       </c>
       <c r="D34" t="n">
-        <v>20</v>
+        <v>18.51</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="n">
-        <v>44963</v>
+        <v>44956.84309027778</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>264.01674599</v>
+        <v>288.44870791</v>
       </c>
       <c r="D35" t="n">
         <v>18.51</v>
@@ -1060,7 +1060,7 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="n">
-        <v>44956</v>
+        <v>44949.78057870371</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>288.44870791</v>
+        <v>265.38112392</v>
       </c>
       <c r="D36" t="n">
         <v>18.51</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="37">
       <c r="A37" s="4" t="n">
-        <v>44949</v>
+        <v>44946.91366898148</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1084,15 +1084,15 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>265.38112392</v>
+        <v>6746.06763447</v>
       </c>
       <c r="D37" t="n">
-        <v>18.51</v>
+        <v>513.26</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="n">
-        <v>44946</v>
+        <v>44942.81034722222</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1100,15 +1100,15 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>6746.06763447</v>
+        <v>372.58940273</v>
       </c>
       <c r="D38" t="n">
-        <v>513.26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="n">
-        <v>44942</v>
+        <v>44937.76524305555</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1116,15 +1116,15 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>372.58940273</v>
+        <v>872.76773121</v>
       </c>
       <c r="D39" t="n">
-        <v>20</v>
+        <v>38.93</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="n">
-        <v>44937</v>
+        <v>44937.76501157408</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1132,15 +1132,15 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>872.76773121</v>
+        <v>655.50684043</v>
       </c>
       <c r="D40" t="n">
-        <v>38.93</v>
+        <v>29.23</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="n">
-        <v>44937</v>
+        <v>44937.76446759259</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1148,15 +1148,15 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>655.50684043</v>
+        <v>656.21331996</v>
       </c>
       <c r="D41" t="n">
-        <v>29.23</v>
+        <v>29.24</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="n">
-        <v>44937</v>
+        <v>44935.6687037037</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1164,47 +1164,47 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>656.21331996</v>
+        <v>443.1084391</v>
       </c>
       <c r="D42" t="n">
-        <v>29.24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="4" t="n">
-        <v>44935</v>
+        <v>44893.29744212963</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>ETH</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>443.1084391</v>
+        <v>0.0003157799999999981</v>
       </c>
       <c r="D43" t="n">
-        <v>20</v>
+        <v>0.3499999999999979</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="n">
-        <v>44893</v>
+        <v>44867.11673611111</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ETH</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.0003157799999999981</v>
+        <v>839.14913695</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3499999999999979</v>
+        <v>48.73</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="n">
-        <v>44867</v>
+        <v>44867.11646990741</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1212,25 +1212,9 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>839.14913695</v>
+        <v>839.61242671</v>
       </c>
       <c r="D45" t="n">
-        <v>48.73</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="4" t="n">
-        <v>44867</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>HBAR</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>839.61242671</v>
-      </c>
-      <c r="D46" t="n">
         <v>48.74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add sell(), sell.json, load.py
</commit_message>
<xml_diff>
--- a/workbooks/after-sales.xlsx
+++ b/workbooks/after-sales.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,10 +505,15 @@
       </c>
       <c r="C1" s="2" t="inlineStr">
         <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Cost Basis</t>
         </is>
@@ -524,9 +529,12 @@
         </is>
       </c>
       <c r="C2" t="n">
+        <v>0.5448788169564495</v>
+      </c>
+      <c r="D2" t="n">
         <v>3616.65739</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>1970.64</v>
       </c>
     </row>
@@ -540,9 +548,12 @@
         </is>
       </c>
       <c r="C3" t="n">
+        <v>0.06803486902880881</v>
+      </c>
+      <c r="D3" t="n">
         <v>10.87677555</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.74</v>
       </c>
     </row>
@@ -556,9 +567,12 @@
         </is>
       </c>
       <c r="C4" t="n">
+        <v>0.07333113036895253</v>
+      </c>
+      <c r="D4" t="n">
         <v>72.68400164000001</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>5.33</v>
       </c>
     </row>
@@ -572,9 +586,12 @@
         </is>
       </c>
       <c r="C5" t="n">
+        <v>0.08702114026711345</v>
+      </c>
+      <c r="D5" t="n">
         <v>34.12963782</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>2.97</v>
       </c>
     </row>
@@ -588,9 +605,12 @@
         </is>
       </c>
       <c r="C6" t="n">
+        <v>0.06583444599568089</v>
+      </c>
+      <c r="D6" t="n">
         <v>48.30298109</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>3.18</v>
       </c>
     </row>
@@ -604,9 +624,12 @@
         </is>
       </c>
       <c r="C7" t="n">
+        <v>0.06109126144076911</v>
+      </c>
+      <c r="D7" t="n">
         <v>10.96719865</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.67</v>
       </c>
     </row>
@@ -620,9 +643,12 @@
         </is>
       </c>
       <c r="C8" t="n">
+        <v>0.06220576971199036</v>
+      </c>
+      <c r="D8" t="n">
         <v>55.78260692</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>3.47</v>
       </c>
     </row>
@@ -636,9 +662,12 @@
         </is>
       </c>
       <c r="C9" t="n">
+        <v>1.00028758268002</v>
+      </c>
+      <c r="D9" t="n">
         <v>0.159954</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.16</v>
       </c>
     </row>
@@ -652,9 +681,12 @@
         </is>
       </c>
       <c r="C10" t="n">
+        <v>0.05164678344993132</v>
+      </c>
+      <c r="D10" t="n">
         <v>15.68345492</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>0.8100000000000001</v>
       </c>
     </row>
@@ -668,9 +700,12 @@
         </is>
       </c>
       <c r="C11" t="n">
+        <v>0.04581990110018071</v>
+      </c>
+      <c r="D11" t="n">
         <v>297.4689965</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>13.63</v>
       </c>
     </row>
@@ -684,9 +719,12 @@
         </is>
       </c>
       <c r="C12" t="n">
+        <v>0.05645797071004285</v>
+      </c>
+      <c r="D12" t="n">
         <v>470.261323</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>26.55</v>
       </c>
     </row>
@@ -700,9 +738,12 @@
         </is>
       </c>
       <c r="C13" t="n">
+        <v>0.0584899292712627</v>
+      </c>
+      <c r="D13" t="n">
         <v>43801.36281517</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>2561.94</v>
       </c>
     </row>
@@ -716,9 +757,12 @@
         </is>
       </c>
       <c r="C14" t="n">
+        <v>0.704848484832252</v>
+      </c>
+      <c r="D14" t="n">
         <v>1418.744626</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -732,9 +776,12 @@
         </is>
       </c>
       <c r="C15" t="n">
+        <v>0.7312994935923857</v>
+      </c>
+      <c r="D15" t="n">
         <v>922.768313</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>674.8200000000001</v>
       </c>
     </row>
@@ -748,9 +795,12 @@
         </is>
       </c>
       <c r="C16" t="n">
+        <v>0.7241962123126896</v>
+      </c>
+      <c r="D16" t="n">
         <v>941.043309</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>681.5</v>
       </c>
     </row>
@@ -764,9 +814,12 @@
         </is>
       </c>
       <c r="C17" t="n">
+        <v>0.7469625014359766</v>
+      </c>
+      <c r="D17" t="n">
         <v>971.856015</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>725.9400000000001</v>
       </c>
     </row>
@@ -780,9 +833,12 @@
         </is>
       </c>
       <c r="C18" t="n">
+        <v>0.0484474033023344</v>
+      </c>
+      <c r="D18" t="n">
         <v>130.2443386</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>6.31</v>
       </c>
     </row>
@@ -796,9 +852,12 @@
         </is>
       </c>
       <c r="C19" t="n">
+        <v>0.05301888793675442</v>
+      </c>
+      <c r="D19" t="n">
         <v>58.46972882</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>3.1</v>
       </c>
     </row>
@@ -812,9 +871,12 @@
         </is>
       </c>
       <c r="C20" t="n">
+        <v>0.0513950184195149</v>
+      </c>
+      <c r="D20" t="n">
         <v>283.8796531</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>14.59</v>
       </c>
     </row>
@@ -828,9 +890,12 @@
         </is>
       </c>
       <c r="C21" t="n">
+        <v>0.428976624570404</v>
+      </c>
+      <c r="D21" t="n">
         <v>44.590986</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>19.13</v>
       </c>
     </row>
@@ -844,9 +909,12 @@
         </is>
       </c>
       <c r="C22" t="n">
+        <v>0.4503605885935721</v>
+      </c>
+      <c r="D22" t="n">
         <v>113.287</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>51.02</v>
       </c>
     </row>
@@ -860,9 +928,12 @@
         </is>
       </c>
       <c r="C23" t="n">
+        <v>0.05890923103526676</v>
+      </c>
+      <c r="D23" t="n">
         <v>6.45060194</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>0.38</v>
       </c>
     </row>
@@ -876,9 +947,12 @@
         </is>
       </c>
       <c r="C24" t="n">
+        <v>0.4801375295817313</v>
+      </c>
+      <c r="D24" t="n">
         <v>2066.699516</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>992.3</v>
       </c>
     </row>
@@ -892,9 +966,12 @@
         </is>
       </c>
       <c r="C25" t="n">
+        <v>0.4488356714405042</v>
+      </c>
+      <c r="D25" t="n">
         <v>805.484107</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>361.53</v>
       </c>
     </row>
@@ -908,9 +985,12 @@
         </is>
       </c>
       <c r="C26" t="n">
+        <v>0.4546727091699747</v>
+      </c>
+      <c r="D26" t="n">
         <v>219.938426</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>100</v>
       </c>
     </row>
@@ -924,9 +1004,12 @@
         </is>
       </c>
       <c r="C27" t="n">
+        <v>0.4371946406745632</v>
+      </c>
+      <c r="D27" t="n">
         <v>1152.377951</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>503.82</v>
       </c>
     </row>
@@ -940,9 +1023,12 @@
         </is>
       </c>
       <c r="C28" t="n">
+        <v>0.06300502512508706</v>
+      </c>
+      <c r="D28" t="n">
         <v>317.43499761</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>20</v>
       </c>
     </row>
@@ -956,9 +1042,12 @@
         </is>
       </c>
       <c r="C29" t="n">
+        <v>0.06458291457213151</v>
+      </c>
+      <c r="D29" t="n">
         <v>309.67942733</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>20</v>
       </c>
     </row>
@@ -972,9 +1061,12 @@
         </is>
       </c>
       <c r="C30" t="n">
+        <v>0.05924242424243397</v>
+      </c>
+      <c r="D30" t="n">
         <v>10127.87723785</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>600</v>
       </c>
     </row>
@@ -988,9 +1080,12 @@
         </is>
       </c>
       <c r="C31" t="n">
+        <v>0.06411055276443217</v>
+      </c>
+      <c r="D31" t="n">
         <v>311.96112243</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1004,9 +1099,12 @@
         </is>
       </c>
       <c r="C32" t="n">
+        <v>0.0690242930183286</v>
+      </c>
+      <c r="D32" t="n">
         <v>12639.46303323</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>872.4299999999999</v>
       </c>
     </row>
@@ -1020,9 +1118,12 @@
         </is>
       </c>
       <c r="C33" t="n">
+        <v>0.07290452261403836</v>
+      </c>
+      <c r="D33" t="n">
         <v>274.33140336</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1036,9 +1137,12 @@
         </is>
       </c>
       <c r="C34" t="n">
+        <v>0.07010918921294899</v>
+      </c>
+      <c r="D34" t="n">
         <v>264.01674599</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>18.51</v>
       </c>
     </row>
@@ -1052,9 +1156,12 @@
         </is>
       </c>
       <c r="C35" t="n">
+        <v>0.06417085427117038</v>
+      </c>
+      <c r="D35" t="n">
         <v>288.44870791</v>
       </c>
-      <c r="D35" t="n">
+      <c r="E35" t="n">
         <v>18.51</v>
       </c>
     </row>
@@ -1068,9 +1175,12 @@
         </is>
       </c>
       <c r="C36" t="n">
+        <v>0.06974874371841119</v>
+      </c>
+      <c r="D36" t="n">
         <v>265.38112392</v>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>18.51</v>
       </c>
     </row>
@@ -1084,9 +1194,12 @@
         </is>
       </c>
       <c r="C37" t="n">
+        <v>0.07608365565557711</v>
+      </c>
+      <c r="D37" t="n">
         <v>6746.06763447</v>
       </c>
-      <c r="D37" t="n">
+      <c r="E37" t="n">
         <v>513.26</v>
       </c>
     </row>
@@ -1100,9 +1213,12 @@
         </is>
       </c>
       <c r="C38" t="n">
+        <v>0.05367839196031339</v>
+      </c>
+      <c r="D38" t="n">
         <v>372.58940273</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1116,9 +1232,12 @@
         </is>
       </c>
       <c r="C39" t="n">
+        <v>0.04459995351554337</v>
+      </c>
+      <c r="D39" t="n">
         <v>872.76773121</v>
       </c>
-      <c r="D39" t="n">
+      <c r="E39" t="n">
         <v>38.93</v>
       </c>
     </row>
@@ -1132,9 +1251,12 @@
         </is>
       </c>
       <c r="C40" t="n">
+        <v>0.04459144923770082</v>
+      </c>
+      <c r="D40" t="n">
         <v>655.50684043</v>
       </c>
-      <c r="D40" t="n">
+      <c r="E40" t="n">
         <v>29.23</v>
       </c>
     </row>
@@ -1148,9 +1270,12 @@
         </is>
       </c>
       <c r="C41" t="n">
+        <v>0.04455868101211714</v>
+      </c>
+      <c r="D41" t="n">
         <v>656.21331996</v>
       </c>
-      <c r="D41" t="n">
+      <c r="E41" t="n">
         <v>29.24</v>
       </c>
     </row>
@@ -1164,9 +1289,12 @@
         </is>
       </c>
       <c r="C42" t="n">
+        <v>0.04513567839200289</v>
+      </c>
+      <c r="D42" t="n">
         <v>443.1084391</v>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1180,9 +1308,12 @@
         </is>
       </c>
       <c r="C43" t="n">
+        <v>1178.442052468954</v>
+      </c>
+      <c r="D43" t="n">
         <v>0.0003157799999999981</v>
       </c>
-      <c r="D43" t="n">
+      <c r="E43" t="n">
         <v>0.3499999999999979</v>
       </c>
     </row>
@@ -1196,9 +1327,12 @@
         </is>
       </c>
       <c r="C44" t="n">
+        <v>0.05807072647076265</v>
+      </c>
+      <c r="D44" t="n">
         <v>839.14913695</v>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>48.73</v>
       </c>
     </row>
@@ -1212,9 +1346,12 @@
         </is>
       </c>
       <c r="C45" t="n">
+        <v>0.05805059388054373</v>
+      </c>
+      <c r="D45" t="n">
         <v>839.61242671</v>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>48.74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add sold, read_f8949, write_f8949
</commit_message>
<xml_diff>
--- a/workbooks/after-sales.xlsx
+++ b/workbooks/after-sales.xlsx
@@ -484,7 +484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,7 +535,7 @@
         <v>3616.65739</v>
       </c>
       <c r="E2" t="n">
-        <v>1970.64</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3">
@@ -741,34 +741,34 @@
         <v>0.0584899292712627</v>
       </c>
       <c r="D13" t="n">
-        <v>43801.36281517</v>
+        <v>43834.38366132</v>
       </c>
       <c r="E13" t="n">
-        <v>2561.94</v>
+        <v>2563.87</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="n">
-        <v>45131.44159722222</v>
+        <v>45146.03059027778</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.704848484832252</v>
+        <v>0.05909090908667258</v>
       </c>
       <c r="D14" t="n">
-        <v>1418.744626</v>
+        <v>53.64615385</v>
       </c>
       <c r="E14" t="n">
-        <v>1000</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="n">
-        <v>45124.80702546296</v>
+        <v>45131.44159722222</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -776,18 +776,18 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.7312994935923857</v>
+        <v>0.704848484832252</v>
       </c>
       <c r="D15" t="n">
-        <v>922.768313</v>
+        <v>1418.744626</v>
       </c>
       <c r="E15" t="n">
-        <v>674.8200000000001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="n">
-        <v>45124.77539351852</v>
+        <v>45124.80702546296</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -795,18 +795,18 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.7241962123126896</v>
+        <v>0.7312994935923857</v>
       </c>
       <c r="D16" t="n">
-        <v>941.043309</v>
+        <v>922.768313</v>
       </c>
       <c r="E16" t="n">
-        <v>681.5</v>
+        <v>674.8200000000001</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="n">
-        <v>45124.75659722222</v>
+        <v>45124.77539351852</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -814,37 +814,37 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.7469625014359766</v>
+        <v>0.7241962123126896</v>
       </c>
       <c r="D17" t="n">
-        <v>971.856015</v>
+        <v>941.043309</v>
       </c>
       <c r="E17" t="n">
-        <v>725.9400000000001</v>
+        <v>681.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="n">
-        <v>45087.11783564815</v>
+        <v>45124.75659722222</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.0484474033023344</v>
+        <v>0.7469625014359766</v>
       </c>
       <c r="D18" t="n">
-        <v>130.2443386</v>
+        <v>971.856015</v>
       </c>
       <c r="E18" t="n">
-        <v>6.31</v>
+        <v>725.9400000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="n">
-        <v>45067.3153125</v>
+        <v>45087.11783564815</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -852,18 +852,18 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.05301888793675442</v>
+        <v>0.0484474033023344</v>
       </c>
       <c r="D19" t="n">
-        <v>58.46972882</v>
+        <v>130.2443386</v>
       </c>
       <c r="E19" t="n">
-        <v>3.1</v>
+        <v>6.31</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="n">
-        <v>45058.33905092593</v>
+        <v>45067.3153125</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -871,37 +871,37 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.0513950184195149</v>
+        <v>0.05301888793675442</v>
       </c>
       <c r="D20" t="n">
-        <v>283.8796531</v>
+        <v>58.46972882</v>
       </c>
       <c r="E20" t="n">
-        <v>14.59</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="n">
-        <v>45058.19652777778</v>
+        <v>45058.33905092593</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.428976624570404</v>
+        <v>0.0513950184195149</v>
       </c>
       <c r="D21" t="n">
-        <v>44.590986</v>
+        <v>283.8796531</v>
       </c>
       <c r="E21" t="n">
-        <v>19.13</v>
+        <v>14.59</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="n">
-        <v>45054.77490740741</v>
+        <v>45058.19652777778</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -909,56 +909,56 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.4503605885935721</v>
+        <v>0.428976624570404</v>
       </c>
       <c r="D22" t="n">
-        <v>113.287</v>
+        <v>44.590986</v>
       </c>
       <c r="E22" t="n">
-        <v>51.02</v>
+        <v>19.13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="n">
-        <v>45014.81280092592</v>
+        <v>45054.77490740741</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.05890923103526676</v>
+        <v>0.4503605885935721</v>
       </c>
       <c r="D23" t="n">
-        <v>6.45060194</v>
+        <v>113.287</v>
       </c>
       <c r="E23" t="n">
-        <v>0.38</v>
+        <v>51.02</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="n">
-        <v>45013.15342592593</v>
+        <v>45014.81280092592</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>XRP</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.4801375295817313</v>
+        <v>0.05890923103526676</v>
       </c>
       <c r="D24" t="n">
-        <v>2066.699516</v>
+        <v>6.45060194</v>
       </c>
       <c r="E24" t="n">
-        <v>992.3</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="n">
-        <v>45012.1265162037</v>
+        <v>45013.15342592593</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -966,18 +966,18 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.4488356714405042</v>
+        <v>0.4801375295817313</v>
       </c>
       <c r="D25" t="n">
-        <v>805.484107</v>
+        <v>2066.699516</v>
       </c>
       <c r="E25" t="n">
-        <v>361.53</v>
+        <v>992.3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="n">
-        <v>45010.50967592592</v>
+        <v>45012.1265162037</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -985,18 +985,18 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.4546727091699747</v>
+        <v>0.4488356714405042</v>
       </c>
       <c r="D26" t="n">
-        <v>219.938426</v>
+        <v>805.484107</v>
       </c>
       <c r="E26" t="n">
-        <v>100</v>
+        <v>361.53</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="n">
-        <v>45006.65659722222</v>
+        <v>45010.50967592592</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1004,37 +1004,37 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.4371946406745632</v>
+        <v>0.4546727091699747</v>
       </c>
       <c r="D27" t="n">
-        <v>1152.377951</v>
+        <v>219.938426</v>
       </c>
       <c r="E27" t="n">
-        <v>503.82</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="n">
-        <v>45005.71923611111</v>
+        <v>45006.65659722222</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>XRP</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.06300502512508706</v>
+        <v>0.4371946406745632</v>
       </c>
       <c r="D28" t="n">
-        <v>317.43499761</v>
+        <v>1152.377951</v>
       </c>
       <c r="E28" t="n">
-        <v>20</v>
+        <v>503.82</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="n">
-        <v>44998.83645833333</v>
+        <v>45005.71923611111</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1042,10 +1042,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.06458291457213151</v>
+        <v>0.06300502512508706</v>
       </c>
       <c r="D29" t="n">
-        <v>309.67942733</v>
+        <v>317.43499761</v>
       </c>
       <c r="E29" t="n">
         <v>20</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="n">
-        <v>44995.76827546296</v>
+        <v>44998.83645833333</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1061,18 +1061,18 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.05924242424243397</v>
+        <v>0.06458291457213151</v>
       </c>
       <c r="D30" t="n">
-        <v>10127.87723785</v>
+        <v>309.67942733</v>
       </c>
       <c r="E30" t="n">
-        <v>600</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="n">
-        <v>44991.70733796297</v>
+        <v>44995.76827546296</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1080,18 +1080,18 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.06411055276443217</v>
+        <v>0.05924242424243397</v>
       </c>
       <c r="D31" t="n">
-        <v>311.96112243</v>
+        <v>10127.87723785</v>
       </c>
       <c r="E31" t="n">
-        <v>20</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="n">
-        <v>44987.0953125</v>
+        <v>44991.70733796297</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1099,18 +1099,18 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.0690242930183286</v>
+        <v>0.06411055276443217</v>
       </c>
       <c r="D32" t="n">
-        <v>12639.46303323</v>
+        <v>311.96112243</v>
       </c>
       <c r="E32" t="n">
-        <v>872.4299999999999</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="n">
-        <v>44984.69497685185</v>
+        <v>44987.0953125</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1118,18 +1118,18 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.07290452261403836</v>
+        <v>0.0690242930183286</v>
       </c>
       <c r="D33" t="n">
-        <v>274.33140336</v>
+        <v>12639.46303323</v>
       </c>
       <c r="E33" t="n">
-        <v>20</v>
+        <v>872.4299999999999</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="n">
-        <v>44963.71480324074</v>
+        <v>44984.69497685185</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1137,18 +1137,18 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.07010918921294899</v>
+        <v>0.07290452261403836</v>
       </c>
       <c r="D34" t="n">
-        <v>264.01674599</v>
+        <v>274.33140336</v>
       </c>
       <c r="E34" t="n">
-        <v>18.51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="n">
-        <v>44956.84309027778</v>
+        <v>44963.71480324074</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1156,18 +1156,18 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.06417085427117038</v>
+        <v>0.07010918921294899</v>
       </c>
       <c r="D35" t="n">
-        <v>288.44870791</v>
+        <v>264.01674599</v>
       </c>
       <c r="E35" t="n">
-        <v>18.51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="n">
-        <v>44949.78057870371</v>
+        <v>44956.84309027778</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1175,18 +1175,18 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.06974874371841119</v>
+        <v>0.06417085427117038</v>
       </c>
       <c r="D36" t="n">
-        <v>265.38112392</v>
+        <v>288.44870791</v>
       </c>
       <c r="E36" t="n">
-        <v>18.51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="n">
-        <v>44946.91366898148</v>
+        <v>44949.78057870371</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1194,18 +1194,18 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.07608365565557711</v>
+        <v>0.06974874371841119</v>
       </c>
       <c r="D37" t="n">
-        <v>6746.06763447</v>
+        <v>265.38112392</v>
       </c>
       <c r="E37" t="n">
-        <v>513.26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="n">
-        <v>44942.81034722222</v>
+        <v>44946.91366898148</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1213,18 +1213,18 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.05367839196031339</v>
+        <v>0.07608365565557711</v>
       </c>
       <c r="D38" t="n">
-        <v>372.58940273</v>
+        <v>6661.40079847</v>
       </c>
       <c r="E38" t="n">
-        <v>20</v>
+        <v>506.82</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="n">
-        <v>44937.76524305555</v>
+        <v>44942.81034722222</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1232,18 +1232,18 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.04459995351554337</v>
+        <v>0.05367839196031339</v>
       </c>
       <c r="D39" t="n">
-        <v>872.76773121</v>
+        <v>372.58940273</v>
       </c>
       <c r="E39" t="n">
-        <v>38.93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="n">
-        <v>44937.76501157408</v>
+        <v>44937.76524305555</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1251,18 +1251,18 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.04459144923770082</v>
+        <v>0.04459995351554337</v>
       </c>
       <c r="D40" t="n">
-        <v>655.50684043</v>
+        <v>872.76773121</v>
       </c>
       <c r="E40" t="n">
-        <v>29.23</v>
+        <v>38.93</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="n">
-        <v>44937.76446759259</v>
+        <v>44937.76501157408</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1270,18 +1270,18 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.04455868101211714</v>
+        <v>0.04459144923770082</v>
       </c>
       <c r="D41" t="n">
-        <v>656.21331996</v>
+        <v>655.50684043</v>
       </c>
       <c r="E41" t="n">
-        <v>29.24</v>
+        <v>29.23</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="n">
-        <v>44935.6687037037</v>
+        <v>44937.76446759259</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1289,69 +1289,88 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.04513567839200289</v>
+        <v>0.04455868101211714</v>
       </c>
       <c r="D42" t="n">
-        <v>443.1084391</v>
+        <v>656.21331996</v>
       </c>
       <c r="E42" t="n">
-        <v>20</v>
+        <v>29.24</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="4" t="n">
-        <v>44893.29744212963</v>
+        <v>44935.6687037037</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ETH</t>
+          <t>HBAR</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1178.442052468954</v>
+        <v>0.04513567839200289</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0003157799999999981</v>
+        <v>443.1084391</v>
       </c>
       <c r="E43" t="n">
-        <v>0.3499999999999979</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="n">
-        <v>44867.11673611111</v>
+        <v>44893.29744212963</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>HBAR</t>
+          <t>ETH</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.05807072647076265</v>
+        <v>1178.442052468954</v>
       </c>
       <c r="D44" t="n">
-        <v>839.14913695</v>
+        <v>0.0003157799999999981</v>
       </c>
       <c r="E44" t="n">
-        <v>48.73</v>
+        <v>0.3499999999999979</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="n">
+        <v>44867.11673611111</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>HBAR</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.05807072647076265</v>
+      </c>
+      <c r="D45" t="n">
+        <v>839.14913695</v>
+      </c>
+      <c r="E45" t="n">
+        <v>48.73</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="n">
         <v>44867.11646990741</v>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>HBAR</t>
-        </is>
-      </c>
-      <c r="C45" t="n">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>HBAR</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
         <v>0.05805059388054373</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D46" t="n">
         <v>839.61242671</v>
       </c>
-      <c r="E45" t="n">
+      <c r="E46" t="n">
         <v>48.74</v>
       </c>
     </row>

</xml_diff>